<commit_message>
I don't want to have anything to do with 2.4 anymore
</commit_message>
<xml_diff>
--- a/A2_results_step_2_2.xlsx
+++ b/A2_results_step_2_2.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d63f66d86bcfcc9a/Master Sustainable Energy/3rd Semester/Renewables in electricity markets/Assignment 1/RenewablesInElectricityMarkets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="115_{CD624BA3-5945-42C1-ACA4-98261464F54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="DC_flow_df" sheetId="1" r:id="rId1"/>
-    <sheet name="Ps_nodal_df" r:id="rId5" sheetId="2"/>
-    <sheet name="Po_nodal_df" r:id="rId6" sheetId="3"/>
-    <sheet name="Dk_nodal_df" r:id="rId7" sheetId="4"/>
-    <sheet name="Clearing_df" r:id="rId8" sheetId="5"/>
-    <sheet name="Price_s_df" r:id="rId9" sheetId="6"/>
-    <sheet name="Price_o_df" r:id="rId10" sheetId="7"/>
-    <sheet name="Bid_d_df" r:id="rId11" sheetId="8"/>
-    <sheet name="SW_vs_Prof_df" r:id="rId12" sheetId="9"/>
-    <sheet name="Profit_df" r:id="rId13" sheetId="10"/>
+    <sheet name="Ps_nodal_df" sheetId="2" r:id="rId2"/>
+    <sheet name="Po_nodal_df" sheetId="3" r:id="rId3"/>
+    <sheet name="Dk_nodal_df" sheetId="4" r:id="rId4"/>
+    <sheet name="Clearing_df" sheetId="5" r:id="rId5"/>
+    <sheet name="Price_s_df" sheetId="6" r:id="rId6"/>
+    <sheet name="Price_o_df" sheetId="7" r:id="rId7"/>
+    <sheet name="Bid_d_df" sheetId="8" r:id="rId8"/>
+    <sheet name="SW_vs_Prof_df" sheetId="9" r:id="rId9"/>
+    <sheet name="Profit_df" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>N1</t>
   </si>
@@ -429,14 +429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52CEE1F-2B92-4098-B175-0B5959F09F16}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,124 +456,124 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>197.8333333333333</v>
+        <v>197.83333333333329</v>
       </c>
       <c r="C2">
         <v>237.16666666666663</v>
       </c>
       <c r="D2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>-197.8333333333333</v>
+        <v>-197.83333333333329</v>
       </c>
       <c r="B3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>39.33333333333332</v>
+        <v>39.333333333333321</v>
       </c>
       <c r="D3">
         <v>508.50000000000006</v>
       </c>
       <c r="E3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>-237.16666666666663</v>
       </c>
       <c r="B4">
-        <v>-39.33333333333332</v>
+        <v>-39.333333333333321</v>
       </c>
       <c r="C4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>441.49999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>-0.0</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>-508.50000000000006</v>
       </c>
       <c r="C5">
-        <v>-0.0</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>136.1666666666667</v>
+        <v>136.16666666666671</v>
       </c>
       <c r="F5">
-        <v>-27.66666666666677</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>-27.666666666666771</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>-0.0</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>-0.0</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>-0.0</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>-136.1666666666667</v>
+        <v>-136.16666666666671</v>
       </c>
       <c r="E6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>-163.83333333333348</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>-0.0</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>-0.0</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>-441.49999999999994</v>
       </c>
       <c r="D7">
-        <v>27.66666666666677</v>
+        <v>27.666666666666771</v>
       </c>
       <c r="E7">
         <v>163.83333333333348</v>
       </c>
       <c r="F7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -582,36 +582,36 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B21CED7-5CF5-41F8-AF73-C58771DBA7C5}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>711.7499999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>711.74999999999977</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>-0.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1131.5</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -620,14 +620,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CC41FC-E629-43B8-B59F-7B9D42A6711C}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,24 +647,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>97.49999999999991</v>
+        <v>97.499999999999915</v>
       </c>
       <c r="B2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>155.0</v>
+        <v>155</v>
       </c>
       <c r="D2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -673,14 +673,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93197726-F956-4CE0-9C29-195F543E2C9E}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -700,24 +700,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>337.5</v>
       </c>
       <c r="B2">
-        <v>350.0</v>
+        <v>350</v>
       </c>
       <c r="C2">
-        <v>210.0</v>
+        <v>210</v>
       </c>
       <c r="D2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -726,14 +726,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF45470-15EB-4BF4-9792-31A441B147D4}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -753,24 +753,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="D2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="E2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="F2">
-        <v>250.0</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -779,44 +779,44 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878EE957-A4D0-4B09-BF85-BDACA7623479}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>22.500000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>22.500000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>22.5</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>22.500000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>22.500000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>22.5</v>
       </c>
@@ -827,14 +827,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{257F33DA-9DA9-4FC3-8390-4971ACEC368B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -842,36 +842,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>22.500000000000004</v>
       </c>
       <c r="B2">
-        <v>97.49999999999991</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>97.499999999999915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>22.500000000000007</v>
       </c>
       <c r="B3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>22.5</v>
       </c>
       <c r="B4">
-        <v>155.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>22.5</v>
       </c>
       <c r="B5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -880,14 +880,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5587BFA-08F7-4A0A-BB45-0BA94E753AB6}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -895,36 +895,36 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>337.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>350.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="B4">
-        <v>210.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>24.7</v>
       </c>
       <c r="B5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -933,14 +933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF67C2-202E-47EC-8534-0B3FECC2AB7E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -948,36 +948,36 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>26.5</v>
       </c>
       <c r="B2">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>24.7</v>
       </c>
       <c r="B3">
-        <v>400.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>23.1</v>
       </c>
       <c r="B4">
-        <v>300.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>22.5</v>
       </c>
       <c r="B5">
-        <v>250.0</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -986,14 +986,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B6F593-CBC5-498E-9C4A-FEF4CA36F18E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1001,9 +1001,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>27735.0</v>
+        <v>27735</v>
       </c>
       <c r="B2">
         <v>1843.2499999999998</v>

</xml_diff>